<commit_message>
update new file icon
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Welcome to Keikai Excel-like Demo</t>
   </si>
@@ -71,14 +71,33 @@
     <t> click  in the toolbar</t>
   </si>
   <si>
-    <t> click  in the toolbar</t>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="2" tint="-0.749992370372631"/>
+        <rFont val="keikai-icon"/>
+        <charset val="129"/>
+      </rPr>
+      <t></t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="2" tint="-0.749992370372631"/>
+        <rFont val="keikai-icon"/>
+      </rPr>
+      <t xml:space="preserve"> in the toolbar</t>
+    </r>
+  </si>
+  <si>
+    <t> click</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -202,6 +221,23 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Font Awesome 5 Free"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="keikai-icon"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="keikai-icon"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Font Awesome 5 Free"/>
     </font>
   </fonts>
@@ -274,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -364,11 +400,11 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -405,6 +441,9 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,8 +469,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FF4185F4"/>
       <color rgb="FFFFC003"/>
-      <color rgb="FF4185F4"/>
       <color rgb="FF1F1D69"/>
       <color rgb="FFFF2837"/>
       <color rgb="FFFF2043"/>
@@ -716,7 +755,7 @@
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -755,21 +794,21 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
       <c r="N2" s="24"/>
     </row>
     <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -789,91 +828,91 @@
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
       <c r="N4" s="25"/>
     </row>
     <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="50"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
+      <c r="A5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="54"/>
       <c r="N5" s="25"/>
     </row>
     <row r="6" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
       <c r="N6" s="25"/>
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="54"/>
       <c r="N7" s="25"/>
     </row>
     <row r="8" spans="1:21" ht="25" x14ac:dyDescent="0.15">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="52" t="s">
+      <c r="H8" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
       <c r="N8" s="26"/>
     </row>
     <row r="9" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -913,14 +952,16 @@
       <c r="N10" s="27"/>
     </row>
     <row r="11" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="32"/>
       <c r="H11" s="37" t="s">
         <v>13</v>
@@ -1182,7 +1223,6 @@
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="H8:M8"/>
     <mergeCell ref="H4:M7"/>
-    <mergeCell ref="A11:F11"/>
     <mergeCell ref="H11:M11"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A10:F10"/>
@@ -1193,6 +1233,7 @@
     <mergeCell ref="H17:M18"/>
     <mergeCell ref="H16:M16"/>
     <mergeCell ref="H14:M15"/>
+    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update welcome.xlsx for links
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="34500" yWindow="460" windowWidth="33600" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome Page" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Welcome to Keikai Excel-like Demo</t>
   </si>
@@ -54,12 +54,6 @@
   </si>
   <si>
     <t>Upload your existing Excel xlsx file</t>
-  </si>
-  <si>
-    <t>Reference tutorial.html or contact us at info@keikai.io</t>
-  </si>
-  <si>
-    <t>Download demo source code from github://URL</t>
   </si>
   <si>
     <t></t>
@@ -122,12 +116,24 @@
       <t xml:space="preserve"> in the toolbar</t>
     </r>
   </si>
+  <si>
+    <t>Download demo source code from</t>
+  </si>
+  <si>
+    <t>github://URL</t>
+  </si>
+  <si>
+    <t>info@keikai.io</t>
+  </si>
+  <si>
+    <t>Reference tutorial.html or contact us at</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -288,6 +294,22 @@
       <sz val="16"/>
       <color theme="2" tint="-0.749992370372631"/>
       <name val="keikai-icon"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="15"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -355,9 +377,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -412,9 +435,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -475,7 +495,6 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -483,6 +502,18 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -512,15 +543,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -528,14 +550,24 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -828,31 +860,33 @@
   </sheetPr>
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:E11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="48" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="2"/>
+    <col min="3" max="3" width="10.6640625" style="44" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="2.1640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="5.83203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="2" customWidth="1"/>
-    <col min="11" max="12" width="14.5" style="2"/>
-    <col min="13" max="14" width="5.83203125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.5" style="2"/>
+    <col min="13" max="13" width="6.83203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.83203125" style="2" customWidth="1"/>
     <col min="15" max="16384" width="14.5" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="35" x14ac:dyDescent="0.15">
       <c r="A1" s="19"/>
       <c r="B1" s="19"/>
-      <c r="C1" s="38"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
@@ -888,12 +922,12 @@
       <c r="K2" s="51"/>
       <c r="L2" s="51"/>
       <c r="M2" s="51"/>
-      <c r="N2" s="23"/>
+      <c r="N2" s="20"/>
     </row>
     <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="39"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -917,14 +951,14 @@
       <c r="F4" s="50"/>
       <c r="G4" s="4"/>
       <c r="H4" s="53" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I4" s="53"/>
       <c r="J4" s="53"/>
       <c r="K4" s="53"/>
       <c r="L4" s="53"/>
       <c r="M4" s="53"/>
-      <c r="N4" s="24"/>
+      <c r="N4" s="21"/>
     </row>
     <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="50"/>
@@ -940,7 +974,7 @@
       <c r="K5" s="53"/>
       <c r="L5" s="53"/>
       <c r="M5" s="53"/>
-      <c r="N5" s="24"/>
+      <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="50"/>
@@ -956,7 +990,7 @@
       <c r="K6" s="53"/>
       <c r="L6" s="53"/>
       <c r="M6" s="53"/>
-      <c r="N6" s="24"/>
+      <c r="N6" s="21"/>
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="50"/>
@@ -972,7 +1006,7 @@
       <c r="K7" s="53"/>
       <c r="L7" s="53"/>
       <c r="M7" s="53"/>
-      <c r="N7" s="24"/>
+      <c r="N7" s="21"/>
     </row>
     <row r="8" spans="1:21" ht="25" x14ac:dyDescent="0.15">
       <c r="A8" s="49" t="s">
@@ -992,23 +1026,23 @@
       <c r="K8" s="52"/>
       <c r="L8" s="52"/>
       <c r="M8" s="52"/>
-      <c r="N8" s="25"/>
+      <c r="N8" s="22"/>
     </row>
     <row r="9" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="26"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="55" t="s">
@@ -1028,36 +1062,36 @@
       <c r="K10" s="56"/>
       <c r="L10" s="56"/>
       <c r="M10" s="56"/>
-      <c r="N10" s="26"/>
+      <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="40" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="64"/>
-      <c r="M11" s="36"/>
-      <c r="N11" s="26"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="62"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="41"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -1068,12 +1102,12 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="27"/>
+      <c r="N12" s="24"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
-      <c r="C13" s="42"/>
+      <c r="C13" s="39"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -1088,7 +1122,7 @@
     </row>
     <row r="14" spans="1:21" ht="93" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="57"/>
       <c r="C14" s="57"/>
@@ -1096,15 +1130,15 @@
       <c r="E14" s="57"/>
       <c r="F14" s="57"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="63" t="s">
+      <c r="H14" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
-      <c r="L14" s="63"/>
-      <c r="M14" s="63"/>
-      <c r="N14" s="28"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="25"/>
     </row>
     <row r="15" spans="1:21" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="57"/>
@@ -1114,13 +1148,13 @@
       <c r="E15" s="57"/>
       <c r="F15" s="57"/>
       <c r="G15" s="12"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63"/>
-      <c r="M15" s="63"/>
-      <c r="N15" s="28"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="25"/>
     </row>
     <row r="16" spans="1:21" ht="25" x14ac:dyDescent="0.15">
       <c r="A16" s="58" t="s">
@@ -1132,51 +1166,55 @@
       <c r="E16" s="58"/>
       <c r="F16" s="58"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="62" t="s">
+      <c r="H16" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="62"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="62"/>
-      <c r="N16" s="25"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="22"/>
     </row>
     <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="54" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="60" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="29"/>
-    </row>
-    <row r="18" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="59"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="26"/>
+    </row>
+    <row r="18" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="63"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="46"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="29"/>
+      <c r="H18" s="64" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="M18" s="65"/>
+      <c r="N18" s="26"/>
     </row>
     <row r="19" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="54"/>
@@ -1186,34 +1224,19 @@
       <c r="E19" s="54"/>
       <c r="F19" s="54"/>
       <c r="G19" s="13"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="29"/>
-    </row>
-    <row r="20" spans="1:14" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="14"/>
-    </row>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="26"/>
+    </row>
+    <row r="20" spans="1:14" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:14" ht="93" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="44"/>
+      <c r="C21" s="40"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
@@ -1229,7 +1252,7 @@
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="45"/>
+      <c r="C22" s="41"/>
       <c r="D22" s="14"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -1245,7 +1268,7 @@
     <row r="23" spans="1:14" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
-      <c r="C23" s="45"/>
+      <c r="C23" s="41"/>
       <c r="D23" s="14"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -1261,7 +1284,7 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
-      <c r="C24" s="44"/>
+      <c r="C24" s="40"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -1277,7 +1300,7 @@
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="17"/>
       <c r="B25" s="17"/>
-      <c r="C25" s="46"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
@@ -1291,32 +1314,38 @@
       <c r="N25" s="17"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="47"/>
+      <c r="C28" s="43"/>
       <c r="D28" s="18"/>
     </row>
     <row r="51" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="H10:M10"/>
     <mergeCell ref="A14:F15"/>
     <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A17:F18"/>
-    <mergeCell ref="H17:M18"/>
     <mergeCell ref="H16:M16"/>
     <mergeCell ref="H14:M15"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="K11:L11"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="L18:M18"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A4:F7"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="H8:M8"/>
     <mergeCell ref="H4:M7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E18" r:id="rId1"/>
+    <hyperlink ref="L18" r:id="rId2"/>
+    <hyperlink ref="M18" r:id="rId3" display="info@keikai.io"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
make a column wider to avoid a new line
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34500" yWindow="460" windowWidth="33600" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome Page" sheetId="2" r:id="rId1"/>
@@ -514,21 +514,6 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,6 +549,21 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -861,7 +861,7 @@
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="129" zoomScaleNormal="129" zoomScalePageLayoutView="129" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F7"/>
+      <selection activeCell="H4" sqref="H4:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -869,14 +869,14 @@
     <col min="1" max="1" width="5.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="44" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="2.1640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="5.83203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="19.1640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" style="2" customWidth="1"/>
     <col min="12" max="12" width="14.5" style="2"/>
     <col min="13" max="13" width="6.83203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="5.83203125" style="2" customWidth="1"/>
@@ -907,21 +907,21 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
       <c r="N2" s="20"/>
     </row>
     <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -941,91 +941,91 @@
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
       <c r="N4" s="21"/>
     </row>
     <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="50"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
+      <c r="A5" s="62"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
       <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
       <c r="N6" s="21"/>
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
       <c r="N7" s="21"/>
     </row>
     <row r="8" spans="1:21" ht="25" x14ac:dyDescent="0.15">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="52" t="s">
+      <c r="H8" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
       <c r="N8" s="22"/>
     </row>
     <row r="9" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1045,23 +1045,23 @@
       <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
       <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -1070,10 +1070,10 @@
       <c r="C11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="61"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="31"/>
       <c r="G11" s="28"/>
       <c r="H11" s="32"/>
@@ -1081,10 +1081,10 @@
       <c r="J11" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="62" t="s">
+      <c r="K11" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="62"/>
+      <c r="L11" s="57"/>
       <c r="M11" s="33"/>
       <c r="N11" s="23"/>
     </row>
@@ -1121,59 +1121,59 @@
       <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:21" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="60" t="s">
+      <c r="H14" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="55"/>
       <c r="N14" s="25"/>
     </row>
     <row r="15" spans="1:21" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
       <c r="G15" s="12"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
+      <c r="M15" s="55"/>
       <c r="N15" s="25"/>
     </row>
     <row r="16" spans="1:21" ht="25" x14ac:dyDescent="0.15">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="59" t="s">
+      <c r="H16" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
       <c r="N16" s="22"/>
     </row>
     <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -1193,36 +1193,36 @@
       <c r="N17" s="26"/>
     </row>
     <row r="18" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
       <c r="E18" s="45" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="46"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="64" t="s">
+      <c r="H18" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="65" t="s">
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="M18" s="65"/>
+      <c r="M18" s="60"/>
       <c r="N18" s="26"/>
     </row>
     <row r="19" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="54"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
       <c r="G19" s="13"/>
       <c r="H19" s="27"/>
       <c r="I19" s="27"/>
@@ -1322,6 +1322,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A4:F7"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="H4:M7"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="H10:M10"/>
@@ -1334,11 +1339,6 @@
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="H18:K18"/>
     <mergeCell ref="L18:M18"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A4:F7"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="H4:M7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E18" r:id="rId1"/>

</xml_diff>

<commit_message>
* change initial focus to row 2 * update github link & tutorial link when the link is ready
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome Page" sheetId="2" r:id="rId1"/>
@@ -65,13 +65,7 @@
     <t>Download demo source code from</t>
   </si>
   <si>
-    <t>github://URL</t>
-  </si>
-  <si>
     <t>info@keikai.io</t>
-  </si>
-  <si>
-    <t>tutorial.html</t>
   </si>
   <si>
     <t xml:space="preserve">Reference </t>
@@ -135,12 +129,18 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>tutorial</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -313,12 +313,6 @@
     <font>
       <u/>
       <sz val="15"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="14"/>
       <color theme="0"/>
       <name val="Arial"/>
     </font>
@@ -566,11 +560,29 @@
     <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -599,29 +611,11 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -920,8 +914,8 @@
   </sheetPr>
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="138" zoomScaleNormal="138" zoomScalePageLayoutView="138" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -973,24 +967,24 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
       <c r="Q2" s="20"/>
     </row>
     <row r="3" spans="1:24" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -1032,106 +1026,106 @@
       <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:24" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="77" t="s">
+      <c r="I5" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
       <c r="Q5" s="21"/>
     </row>
     <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="74"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="77"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="67"/>
+      <c r="P6" s="67"/>
       <c r="Q6" s="21"/>
     </row>
     <row r="7" spans="1:24" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="74"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
       <c r="Q7" s="21"/>
     </row>
     <row r="8" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="74"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="77"/>
-      <c r="P8" s="77"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
       <c r="Q8" s="21"/>
     </row>
     <row r="9" spans="1:24" ht="25" x14ac:dyDescent="0.15">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="76" t="s">
+      <c r="I9" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
+      <c r="J9" s="66"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
       <c r="Q9" s="22"/>
     </row>
     <row r="10" spans="1:24" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1154,58 +1148,58 @@
       <c r="Q10" s="23"/>
     </row>
     <row r="11" spans="1:24" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="64" t="s">
+      <c r="I11" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="64"/>
-      <c r="P11" s="64"/>
+      <c r="J11" s="70"/>
+      <c r="K11" s="70"/>
+      <c r="L11" s="70"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="70"/>
+      <c r="O11" s="70"/>
+      <c r="P11" s="70"/>
       <c r="Q11" s="23"/>
     </row>
     <row r="12" spans="1:24" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="28"/>
       <c r="B12" s="28"/>
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="59" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="46" t="s">
-        <v>21</v>
-      </c>
       <c r="F12" s="58" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G12" s="30"/>
       <c r="H12" s="27"/>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
       <c r="K12" s="56" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L12" s="47" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M12" s="48" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N12" s="50" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O12" s="50"/>
       <c r="P12" s="49"/>
@@ -1257,79 +1251,79 @@
       <c r="F15" s="44"/>
       <c r="G15" s="44"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
-      <c r="K15" s="70"/>
-      <c r="L15" s="70"/>
-      <c r="M15" s="70"/>
-      <c r="N15" s="70"/>
-      <c r="O15" s="70"/>
-      <c r="P15" s="70"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="76"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="76"/>
+      <c r="N15" s="76"/>
+      <c r="O15" s="76"/>
+      <c r="P15" s="76"/>
       <c r="Q15" s="11"/>
     </row>
     <row r="16" spans="1:24" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="68" t="s">
+      <c r="I16" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="68"/>
-      <c r="O16" s="68"/>
-      <c r="P16" s="68"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="74"/>
+      <c r="L16" s="74"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="74"/>
+      <c r="P16" s="74"/>
       <c r="Q16" s="25"/>
     </row>
     <row r="17" spans="1:17" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="65"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="68"/>
-      <c r="N17" s="68"/>
-      <c r="O17" s="68"/>
-      <c r="P17" s="68"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="74"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="74"/>
       <c r="Q17" s="25"/>
     </row>
     <row r="18" spans="1:17" ht="25" x14ac:dyDescent="0.15">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="67" t="s">
+      <c r="I18" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="67"/>
-      <c r="N18" s="67"/>
-      <c r="O18" s="67"/>
-      <c r="P18" s="67"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="73"/>
       <c r="Q18" s="22"/>
     </row>
     <row r="19" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -1352,43 +1346,43 @@
       <c r="Q19" s="26"/>
     </row>
     <row r="20" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="61"/>
-      <c r="B20" s="72" t="s">
+      <c r="A20" s="60"/>
+      <c r="B20" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="60" t="s">
-        <v>12</v>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="62" t="s">
+        <v>21</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="51"/>
       <c r="J20" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="71" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="78"/>
+      <c r="M20" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="L20" s="71"/>
-      <c r="M20" s="69" t="s">
-        <v>16</v>
-      </c>
-      <c r="N20" s="69"/>
+      <c r="N20" s="75"/>
       <c r="O20" s="54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P20" s="51"/>
     </row>
     <row r="21" spans="1:17" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="62"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
+      <c r="A21" s="68"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
       <c r="H21" s="13"/>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
@@ -1506,11 +1500,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A5:G8"/>
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="I9:P9"/>
-    <mergeCell ref="I5:P8"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="I11:P11"/>
@@ -1522,12 +1511,18 @@
     <mergeCell ref="I15:P15"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="B20:F20"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A5:G8"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="I9:P9"/>
+    <mergeCell ref="I5:P8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G20" r:id="rId1"/>
-    <hyperlink ref="K20" r:id="rId2"/>
+    <hyperlink ref="K20" r:id="rId1" display="tutorial.html"/>
+    <hyperlink ref="G20" r:id="rId2"/>
+    <hyperlink ref="L20" r:id="rId3" display="https://github.com/zkoss/keikai-tutorial"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove font awesome font from cells
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -249,12 +249,6 @@
       <charset val="129"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="keikai-icon"/>
-      <charset val="129"/>
-    </font>
-    <font>
       <b/>
       <sz val="60"/>
       <color theme="0"/>
@@ -269,6 +263,12 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -504,27 +504,12 @@
     <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -534,7 +519,7 @@
     <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -543,16 +528,10 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -560,6 +539,27 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1213,21 +1213,21 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
       <c r="N2" s="20"/>
     </row>
     <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -1263,87 +1263,87 @@
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="59"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
       <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="59"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
+      <c r="A6" s="69"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
       <c r="N6" s="21"/>
     </row>
     <row r="7" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="59"/>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
       <c r="N7" s="21"/>
     </row>
     <row r="8" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="59"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
       <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:21" ht="25" x14ac:dyDescent="0.15">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="61" t="s">
+      <c r="H9" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="61"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="71"/>
       <c r="N9" s="22"/>
     </row>
     <row r="10" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1363,23 +1363,23 @@
       <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
       <c r="G11" s="52"/>
-      <c r="H11" s="65" t="s">
+      <c r="H11" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
       <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -1388,10 +1388,10 @@
       <c r="C12" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="70"/>
+      <c r="E12" s="65"/>
       <c r="F12" s="30"/>
       <c r="G12" s="52"/>
       <c r="H12" s="31"/>
@@ -1399,10 +1399,10 @@
       <c r="J12" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="71" t="s">
+      <c r="K12" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="72"/>
+      <c r="L12" s="74"/>
       <c r="M12" s="31"/>
       <c r="N12" s="23"/>
     </row>
@@ -1455,55 +1455,55 @@
       <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:21" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="66"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
       <c r="N16" s="25"/>
     </row>
     <row r="17" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="66"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
       <c r="N17" s="25"/>
     </row>
     <row r="18" spans="1:14" ht="25" x14ac:dyDescent="0.15">
-      <c r="A18" s="67" t="s">
+      <c r="A18" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="68" t="s">
+      <c r="H18" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="68"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
       <c r="N18" s="22"/>
     </row>
     <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -1523,12 +1523,12 @@
       <c r="N19" s="26"/>
     </row>
     <row r="20" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="73"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
       <c r="E20" s="54" t="s">
         <v>15</v>
       </c>
@@ -1544,19 +1544,19 @@
       <c r="K20" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="L20" s="74" t="s">
+      <c r="L20" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="74"/>
+      <c r="M20" s="67"/>
       <c r="N20" s="26"/>
     </row>
     <row r="21" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="63"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
       <c r="G21" s="13"/>
       <c r="H21" s="27"/>
       <c r="I21" s="27"/>
@@ -1656,6 +1656,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A5:F8"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H5:M8"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="H11:M11"/>
@@ -1667,11 +1672,6 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="L20:M20"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A5:F8"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H5:M8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E20" r:id="rId1"/>

</xml_diff>

<commit_message>
update welcome.xlsx for fonts
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/book/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,6 +56,9 @@
     <t>info@keikai.io</t>
   </si>
   <si>
+    <t>tutorial.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reference </t>
   </si>
   <si>
@@ -76,15 +79,12 @@
   <si>
     <t>GitHub</t>
   </si>
-  <si>
-    <t>tutorial</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -185,6 +185,12 @@
       <sz val="24"/>
       <color theme="1" tint="0.249977111117893"/>
       <name val="Arial Bold"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="60"/>
+      <color theme="0"/>
+      <name val="Font Awesome 5 Free"/>
     </font>
     <font>
       <b/>
@@ -228,54 +234,30 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="15"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="60"/>
+      <color theme="0"/>
+      <name val="Abadi MT Condensed Light"/>
+    </font>
+    <font>
       <b/>
+      <sz val="24"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Arial Bold"/>
+    </font>
+    <font>
+      <u/>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="keikai-icon"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="60"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="60"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,12 +279,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF2FB5B6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,9 +325,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -425,25 +401,22 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -453,113 +426,113 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -593,158 +566,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1004186</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>393798</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>780715</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>1168498</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7895659" y="5326124"/>
-          <a:ext cx="774700" cy="774700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>334729</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>403642</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1109429</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>1178342</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2313566" y="5335968"/>
-          <a:ext cx="774700" cy="774700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>984496</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>295349</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>773725</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>130643</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7875969" y="1831163"/>
-          <a:ext cx="774700" cy="800100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>324886</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>315039</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1073104</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>98451</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2303723" y="1850853"/>
-          <a:ext cx="748218" cy="748218"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>143584</xdr:colOff>
       <xdr:row>11</xdr:row>
@@ -764,7 +585,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -802,7 +623,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -822,15 +643,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>219744</xdr:colOff>
+      <xdr:colOff>316692</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>68648</xdr:rowOff>
+      <xdr:rowOff>58953</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>437805</xdr:colOff>
+      <xdr:colOff>534753</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>296616</xdr:rowOff>
+      <xdr:rowOff>286921</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -840,14 +661,14 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7102950" y="3849564"/>
+          <a:off x="7199898" y="3839869"/>
           <a:ext cx="218061" cy="227968"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -878,7 +699,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -887,6 +708,158 @@
         <a:xfrm>
           <a:off x="8110453" y="3818736"/>
           <a:ext cx="268873" cy="268873"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>911298</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>358703</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>758988</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9694</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7794504" y="5312672"/>
+          <a:ext cx="826850" cy="833740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>242367</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>368398</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1056718</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>6786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2220077" y="5322367"/>
+          <a:ext cx="814351" cy="821137"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>261756</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>300533</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1037330</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>106641</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2239466" y="1841983"/>
+          <a:ext cx="775574" cy="775574"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>950076</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>358703</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>759307</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>184198</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7833282" y="1900153"/>
+          <a:ext cx="788391" cy="794961"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1166,25 +1139,25 @@
   </sheetPr>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="131" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="131" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="39" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="2.1640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="6.83203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.5" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="16.83203125" style="2" customWidth="1"/>
     <col min="12" max="12" width="9.33203125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15" style="2" customWidth="1"/>
     <col min="14" max="14" width="5.83203125" style="2" customWidth="1"/>
     <col min="15" max="16384" width="14.5" style="2"/>
   </cols>
@@ -1192,7 +1165,7 @@
     <row r="1" spans="1:21" ht="35" x14ac:dyDescent="0.15">
       <c r="A1" s="19"/>
       <c r="B1" s="19"/>
-      <c r="C1" s="32"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
@@ -1213,27 +1186,27 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
       <c r="N2" s="20"/>
     </row>
     <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="33"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -1247,169 +1220,169 @@
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="69"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
       <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="69"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
       <c r="N6" s="21"/>
     </row>
     <row r="7" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="69"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
       <c r="N7" s="21"/>
     </row>
     <row r="8" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="69"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
       <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:21" ht="25" x14ac:dyDescent="0.15">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="71" t="s">
+      <c r="H9" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="71"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
       <c r="N9" s="22"/>
     </row>
     <row r="10" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
       <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="60" t="s">
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
       <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="65" t="s">
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="65"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="57" t="s">
+      <c r="D12" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="73" t="s">
+      <c r="E12" s="64"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="74"/>
-      <c r="M12" s="31"/>
+      <c r="K12" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="70"/>
+      <c r="M12" s="30"/>
       <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="34"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -1425,7 +1398,7 @@
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="35"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -1439,138 +1412,138 @@
       <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="46"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
       <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:21" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="61"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="64"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="69"/>
       <c r="N16" s="25"/>
     </row>
     <row r="17" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="61"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="64"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="69"/>
+      <c r="L17" s="69"/>
+      <c r="M17" s="69"/>
       <c r="N17" s="25"/>
     </row>
     <row r="18" spans="1:14" ht="25" x14ac:dyDescent="0.15">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="63" t="s">
+      <c r="H18" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="63"/>
-      <c r="L18" s="63"/>
-      <c r="M18" s="63"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
       <c r="N18" s="22"/>
     </row>
     <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
       <c r="G19" s="13"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="43"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
       <c r="N19" s="26"/>
     </row>
     <row r="20" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="54" t="s">
-        <v>15</v>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="73" t="s">
+        <v>16</v>
       </c>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51" t="s">
+      <c r="F20" s="46"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="55" t="s">
-        <v>16</v>
+      <c r="K20" s="52" t="s">
+        <v>11</v>
       </c>
-      <c r="K20" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="L20" s="67" t="s">
+      <c r="L20" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="67"/>
+      <c r="M20" s="72"/>
       <c r="N20" s="26"/>
     </row>
     <row r="21" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="58"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
       <c r="N21" s="26"/>
     </row>
     <row r="22" spans="1:14" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:14" ht="93" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
-      <c r="C23" s="36"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
@@ -1586,7 +1559,7 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
-      <c r="C24" s="37"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="14"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -1602,7 +1575,7 @@
     <row r="25" spans="1:14" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="37"/>
+      <c r="C25" s="36"/>
       <c r="D25" s="14"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -1618,7 +1591,7 @@
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
-      <c r="C26" s="36"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
@@ -1634,7 +1607,7 @@
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
-      <c r="C27" s="38"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
@@ -1648,7 +1621,7 @@
       <c r="N27" s="17"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="39"/>
+      <c r="C30" s="38"/>
       <c r="D30" s="18"/>
     </row>
     <row r="53" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1656,11 +1629,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A5:F8"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H5:M8"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="H11:M11"/>
@@ -1672,12 +1640,17 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="L20:M20"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A5:F8"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H5:M8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E20" r:id="rId1"/>
-    <hyperlink ref="L20" r:id="rId2"/>
-    <hyperlink ref="M20" r:id="rId3" display="info@keikai.io"/>
-    <hyperlink ref="J20" r:id="rId4"/>
+    <hyperlink ref="L20" r:id="rId1"/>
+    <hyperlink ref="M20" r:id="rId2" display="info@keikai.io"/>
+    <hyperlink ref="J20" r:id="rId3"/>
+    <hyperlink ref="E20" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>

</xml_diff>

<commit_message>
update welcome.xlsx for github link
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -483,23 +483,8 @@
     <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -531,8 +516,23 @@
     <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1139,8 +1139,8 @@
   </sheetPr>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="131" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="131" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1186,21 +1186,21 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
       <c r="N2" s="20"/>
     </row>
     <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -1236,87 +1236,87 @@
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="73"/>
+      <c r="L5" s="73"/>
+      <c r="M5" s="73"/>
       <c r="N5" s="21"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="58"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
+      <c r="A6" s="69"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
       <c r="N6" s="21"/>
     </row>
     <row r="7" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="58"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
+      <c r="A7" s="69"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
       <c r="N7" s="21"/>
     </row>
     <row r="8" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="58"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="M8" s="73"/>
       <c r="N8" s="21"/>
     </row>
     <row r="9" spans="1:21" ht="25" x14ac:dyDescent="0.15">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="61" t="s">
+      <c r="H9" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="61"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
       <c r="N9" s="22"/>
     </row>
     <row r="10" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1336,23 +1336,23 @@
       <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
       <c r="G11" s="48"/>
-      <c r="H11" s="65" t="s">
+      <c r="H11" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
       <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -1361,10 +1361,10 @@
       <c r="C12" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="64"/>
+      <c r="E12" s="59"/>
       <c r="F12" s="29"/>
       <c r="G12" s="48"/>
       <c r="H12" s="30"/>
@@ -1372,10 +1372,10 @@
       <c r="J12" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="70" t="s">
+      <c r="K12" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="70"/>
+      <c r="L12" s="65"/>
       <c r="M12" s="30"/>
       <c r="N12" s="23"/>
     </row>
@@ -1428,55 +1428,55 @@
       <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:21" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="66"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
       <c r="N16" s="25"/>
     </row>
     <row r="17" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="66"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
       <c r="N17" s="25"/>
     </row>
     <row r="18" spans="1:14" ht="25" x14ac:dyDescent="0.15">
-      <c r="A18" s="67" t="s">
+      <c r="A18" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="68" t="s">
+      <c r="H18" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
-      <c r="K18" s="68"/>
-      <c r="L18" s="68"/>
-      <c r="M18" s="68"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
       <c r="N18" s="22"/>
     </row>
     <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -1496,13 +1496,13 @@
       <c r="N19" s="26"/>
     </row>
     <row r="20" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="71" t="s">
+      <c r="A20" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="73" t="s">
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="57" t="s">
         <v>16</v>
       </c>
       <c r="F20" s="46"/>
@@ -1517,19 +1517,19 @@
       <c r="K20" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="72" t="s">
+      <c r="L20" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="72"/>
+      <c r="M20" s="67"/>
       <c r="N20" s="26"/>
     </row>
     <row r="21" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="63"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
+      <c r="A21" s="58"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
       <c r="G21" s="13"/>
       <c r="H21" s="53"/>
       <c r="I21" s="53"/>
@@ -1629,6 +1629,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A5:F8"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H5:M8"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="H11:M11"/>
@@ -1640,11 +1645,6 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="L20:M20"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A5:F8"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H5:M8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L20" r:id="rId1"/>

</xml_diff>

<commit_message>
focus A1 of welcome.xlsx
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -491,6 +491,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -520,24 +538,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1144,9 +1144,7 @@
   </sheetPr>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1191,21 +1189,21 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
       <c r="N2" s="57"/>
     </row>
     <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -1241,87 +1239,87 @@
       <c r="N4" s="57"/>
     </row>
     <row r="5" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="70"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
       <c r="N5" s="20"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="70"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
       <c r="N6" s="20"/>
     </row>
     <row r="7" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="70"/>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
       <c r="N7" s="20"/>
     </row>
     <row r="8" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="70"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
       <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:21" ht="25" x14ac:dyDescent="0.15">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="73" t="s">
+      <c r="H9" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
       <c r="N9" s="21"/>
     </row>
     <row r="10" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1341,23 +1339,23 @@
       <c r="N10" s="22"/>
     </row>
     <row r="11" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
       <c r="G11" s="47"/>
-      <c r="H11" s="61" t="s">
+      <c r="H11" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
       <c r="N11" s="22"/>
     </row>
     <row r="12" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -1366,10 +1364,10 @@
       <c r="C12" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="60"/>
+      <c r="E12" s="66"/>
       <c r="F12" s="28"/>
       <c r="G12" s="47"/>
       <c r="H12" s="29"/>
@@ -1377,10 +1375,10 @@
       <c r="J12" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="66" t="s">
+      <c r="K12" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="66"/>
+      <c r="L12" s="72"/>
       <c r="M12" s="29"/>
       <c r="N12" s="22"/>
     </row>
@@ -1433,55 +1431,55 @@
       <c r="N15" s="23"/>
     </row>
     <row r="16" spans="1:21" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="65"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="71"/>
       <c r="N16" s="24"/>
     </row>
     <row r="17" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
+      <c r="A17" s="68"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="65"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
       <c r="N17" s="24"/>
     </row>
     <row r="18" spans="1:14" ht="25" x14ac:dyDescent="0.15">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="64" t="s">
+      <c r="H18" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="64"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="70"/>
       <c r="N18" s="21"/>
     </row>
     <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -1501,12 +1499,12 @@
       <c r="N19" s="25"/>
     </row>
     <row r="20" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
       <c r="E20" s="56" t="s">
         <v>15</v>
       </c>
@@ -1522,19 +1520,19 @@
       <c r="K20" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="L20" s="68" t="s">
+      <c r="L20" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="68"/>
+      <c r="M20" s="74"/>
       <c r="N20" s="25"/>
     </row>
     <row r="21" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="59"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
       <c r="G21" s="13"/>
       <c r="H21" s="52"/>
       <c r="I21" s="52"/>
@@ -1634,11 +1632,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A5:F8"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H5:M8"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="H11:M11"/>
@@ -1650,6 +1643,11 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="L20:M20"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A5:F8"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H5:M8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L20" r:id="rId1"/>

</xml_diff>

<commit_message>
fix layout & style problems in welcome.xlsx
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/book/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="22700" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome Page" sheetId="2" r:id="rId1"/>
@@ -48,9 +53,6 @@
     <t>info@keikai.io</t>
   </si>
   <si>
-    <t>tutorial.html</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reference </t>
   </si>
   <si>
@@ -74,16 +76,19 @@
   <si>
     <t>Welcome to Keikai Online Editor Demo</t>
   </si>
+  <si>
+    <t>tutorial</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="31">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -203,7 +208,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -243,13 +248,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="24"/>
       <color theme="1" tint="0.249977111117893"/>
@@ -258,9 +256,17 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -328,7 +334,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -409,9 +415,6 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -436,9 +439,6 @@
     <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -481,23 +481,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -529,11 +514,29 @@
     <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -682,7 +685,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>728638</xdr:colOff>
+      <xdr:colOff>817538</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>9694</xdr:rowOff>
     </xdr:to>
@@ -796,7 +799,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>726207</xdr:colOff>
+      <xdr:colOff>777007</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>184198</xdr:rowOff>
     </xdr:to>
@@ -1121,55 +1124,55 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="19.875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="6.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="6.83203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="13" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="2" customWidth="1"/>
     <col min="13" max="13" width="15" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.83203125" style="2" customWidth="1"/>
     <col min="15" max="16384" width="14.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="34.5">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
+    <row r="1" spans="1:21" ht="35" x14ac:dyDescent="0.15">
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1178,148 +1181,148 @@
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
     </row>
-    <row r="2" spans="1:21" ht="47.1" customHeight="1">
-      <c r="A2" s="58" t="s">
-        <v>16</v>
+    <row r="2" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="67" t="s">
+        <v>15</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="42"/>
-    </row>
-    <row r="3" spans="1:21" ht="14.1" customHeight="1">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="42"/>
-    </row>
-    <row r="4" spans="1:21" ht="24.95" customHeight="1">
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="40"/>
+    </row>
+    <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="40"/>
+    </row>
+    <row r="4" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="27"/>
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
-      <c r="G4" s="43"/>
+      <c r="G4" s="41"/>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
       <c r="L4" s="28"/>
       <c r="M4" s="28"/>
-      <c r="N4" s="42"/>
-    </row>
-    <row r="5" spans="1:21" ht="45" customHeight="1">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
+      <c r="N4" s="40"/>
+    </row>
+    <row r="5" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="66"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:21" ht="18" customHeight="1">
-      <c r="A6" s="57"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="61"/>
+    <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="66"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
       <c r="N6" s="10"/>
     </row>
-    <row r="7" spans="1:21" ht="12.95" customHeight="1">
-      <c r="A7" s="57"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
+    <row r="7" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="66"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
       <c r="N7" s="10"/>
     </row>
-    <row r="8" spans="1:21" ht="27" customHeight="1">
-      <c r="A8" s="57"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
+    <row r="8" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="66"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="70"/>
       <c r="N8" s="10"/>
     </row>
-    <row r="9" spans="1:21" ht="26.25">
-      <c r="A9" s="56" t="s">
+    <row r="9" spans="1:21" ht="25" x14ac:dyDescent="0.15">
+      <c r="A9" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="60" t="s">
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:21" ht="24.95" customHeight="1">
+    <row r="10" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="49"/>
+      <c r="G10" s="47"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
@@ -1328,58 +1331,58 @@
       <c r="M10" s="17"/>
       <c r="N10" s="12"/>
     </row>
-    <row r="11" spans="1:21" ht="23.1" customHeight="1">
-      <c r="A11" s="63" t="s">
+    <row r="11" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="64" t="s">
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="64"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
       <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="1:21" ht="29.1" customHeight="1">
-      <c r="A12" s="33"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="38" t="s">
+    <row r="12" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="E12" s="56"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="63"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="39" t="s">
+      <c r="K12" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="69" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="69"/>
+      <c r="L12" s="62"/>
       <c r="M12" s="19"/>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="1:21" ht="23.1" customHeight="1">
+    <row r="13" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="20"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="51"/>
+      <c r="G13" s="49"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -1388,14 +1391,14 @@
       <c r="M13" s="4"/>
       <c r="N13" s="13"/>
     </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1">
-      <c r="A14" s="51"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
@@ -1404,14 +1407,14 @@
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
     </row>
-    <row r="15" spans="1:21" ht="24.95" customHeight="1">
+    <row r="15" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="30"/>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
-      <c r="G15" s="51"/>
+      <c r="G15" s="49"/>
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
@@ -1420,120 +1423,120 @@
       <c r="M15" s="31"/>
       <c r="N15" s="13"/>
     </row>
-    <row r="16" spans="1:21" ht="93" customHeight="1">
-      <c r="A16" s="65"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
+    <row r="16" spans="1:21" ht="93" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="58"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
       <c r="N16" s="14"/>
     </row>
-    <row r="17" spans="1:14" ht="21.95" customHeight="1">
-      <c r="A17" s="65"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="68"/>
+    <row r="17" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="61"/>
       <c r="N17" s="14"/>
     </row>
-    <row r="18" spans="1:14" ht="26.25">
-      <c r="A18" s="66" t="s">
+    <row r="18" spans="1:14" ht="25" x14ac:dyDescent="0.15">
+      <c r="A18" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="67" t="s">
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="67"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
       <c r="N18" s="11"/>
     </row>
-    <row r="19" spans="1:14" ht="18" customHeight="1">
+    <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="26"/>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
       <c r="N19" s="15"/>
     </row>
-    <row r="20" spans="1:14" ht="45" customHeight="1">
-      <c r="A20" s="70" t="s">
+    <row r="20" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="70"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="41" t="s">
-        <v>15</v>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="54" t="s">
+        <v>14</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36" t="s">
+      <c r="F20" s="26"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="K20" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="L20" s="71" t="s">
+      <c r="L20" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="71"/>
+      <c r="M20" s="64"/>
       <c r="N20" s="15"/>
     </row>
-    <row r="21" spans="1:14" ht="29.1" customHeight="1">
-      <c r="A21" s="62"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
+    <row r="21" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="55"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
       <c r="N21" s="15"/>
     </row>
-    <row r="22" spans="1:14" customFormat="1" ht="23.1" customHeight="1"/>
-    <row r="23" spans="1:14" ht="93" customHeight="1">
+    <row r="22" spans="1:14" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:14" ht="93" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="21"/>
@@ -1549,7 +1552,7 @@
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="22"/>
@@ -1565,7 +1568,7 @@
       <c r="M24" s="6"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="1:14" ht="35.1" customHeight="1">
+    <row r="25" spans="1:14" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="22"/>
@@ -1581,7 +1584,7 @@
       <c r="M25" s="6"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1">
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="21"/>
@@ -1597,7 +1600,7 @@
       <c r="M26" s="5"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="23"/>
@@ -1613,15 +1616,20 @@
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C30" s="24"/>
       <c r="D30" s="9"/>
     </row>
-    <row r="53" spans="1:1" ht="15.75" customHeight="1">
+    <row r="53" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A5:F8"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H5:M8"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="H11:M11"/>
@@ -1633,17 +1641,12 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="L20:M20"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A5:F8"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H5:M8"/>
   </mergeCells>
-  <phoneticPr fontId="30" type="noConversion"/>
+  <phoneticPr fontId="29" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L20" r:id="rId1"/>
     <hyperlink ref="M20" r:id="rId2" display="info@keikai.io"/>
-    <hyperlink ref="J20" r:id="rId3"/>
+    <hyperlink ref="J20" r:id="rId3" display="tutorial.html"/>
     <hyperlink ref="E20" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
reset zoom level to 100%
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -484,6 +484,24 @@
     <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -513,24 +531,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1137,7 +1137,9 @@
   </sheetPr>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1182,21 +1184,21 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
       <c r="N2" s="40"/>
     </row>
     <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -1232,87 +1234,87 @@
       <c r="N4" s="40"/>
     </row>
     <row r="5" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="66"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
       <c r="G5" s="44"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
       <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="66"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
       <c r="G6" s="45"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
       <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="66"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="45"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="70"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="66"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="45"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
       <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:21" ht="25" x14ac:dyDescent="0.15">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
       <c r="G9" s="46"/>
-      <c r="H9" s="69" t="s">
+      <c r="H9" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="59"/>
       <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1332,23 +1334,23 @@
       <c r="N10" s="12"/>
     </row>
     <row r="11" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
       <c r="G11" s="48"/>
-      <c r="H11" s="57" t="s">
+      <c r="H11" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
       <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -1357,10 +1359,10 @@
       <c r="C12" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="56"/>
+      <c r="E12" s="62"/>
       <c r="F12" s="18"/>
       <c r="G12" s="48"/>
       <c r="H12" s="19"/>
@@ -1368,10 +1370,10 @@
       <c r="J12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="62" t="s">
+      <c r="K12" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="62"/>
+      <c r="L12" s="68"/>
       <c r="M12" s="19"/>
       <c r="N12" s="12"/>
     </row>
@@ -1424,55 +1426,55 @@
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:21" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="58"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
+      <c r="A16" s="64"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
       <c r="G16" s="50"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="61"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
       <c r="N16" s="14"/>
     </row>
     <row r="17" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="58"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
+      <c r="A17" s="64"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
       <c r="G17" s="50"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
       <c r="N17" s="14"/>
     </row>
     <row r="18" spans="1:14" ht="25" x14ac:dyDescent="0.15">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
       <c r="G18" s="46"/>
-      <c r="H18" s="60" t="s">
+      <c r="H18" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="66"/>
       <c r="N18" s="11"/>
     </row>
     <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -1492,12 +1494,12 @@
       <c r="N19" s="15"/>
     </row>
     <row r="20" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
       <c r="E20" s="54" t="s">
         <v>14</v>
       </c>
@@ -1513,19 +1515,19 @@
       <c r="K20" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="64" t="s">
+      <c r="L20" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="64"/>
+      <c r="M20" s="70"/>
       <c r="N20" s="15"/>
     </row>
     <row r="21" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="55"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
       <c r="G21" s="51"/>
       <c r="H21" s="36"/>
       <c r="I21" s="36"/>
@@ -1625,11 +1627,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A5:F8"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H5:M8"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="H11:M11"/>
@@ -1641,6 +1638,11 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="L20:M20"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A5:F8"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H5:M8"/>
   </mergeCells>
   <phoneticPr fontId="29" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
fix Github link's font
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -259,14 +259,6 @@
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -481,27 +473,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -531,6 +502,27 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1137,8 +1129,8 @@
   </sheetPr>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1184,21 +1176,21 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
       <c r="N2" s="40"/>
     </row>
     <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -1234,87 +1226,87 @@
       <c r="N4" s="40"/>
     </row>
     <row r="5" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="56"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
       <c r="G5" s="44"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
       <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="56"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
       <c r="G6" s="45"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
       <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="56"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
       <c r="G7" s="45"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="69"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="56"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
       <c r="G8" s="45"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
       <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:21" ht="25" x14ac:dyDescent="0.15">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
       <c r="G9" s="46"/>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="59"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68"/>
       <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1334,23 +1326,23 @@
       <c r="N10" s="12"/>
     </row>
     <row r="11" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
       <c r="G11" s="48"/>
-      <c r="H11" s="63" t="s">
+      <c r="H11" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="63"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
       <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -1359,10 +1351,10 @@
       <c r="C12" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="62"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="18"/>
       <c r="G12" s="48"/>
       <c r="H12" s="19"/>
@@ -1370,10 +1362,10 @@
       <c r="J12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="68" t="s">
+      <c r="K12" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="68"/>
+      <c r="L12" s="61"/>
       <c r="M12" s="19"/>
       <c r="N12" s="12"/>
     </row>
@@ -1426,55 +1418,55 @@
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:21" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="64"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
       <c r="G16" s="50"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
       <c r="N16" s="14"/>
     </row>
     <row r="17" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="64"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
       <c r="G17" s="50"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="67"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
       <c r="N17" s="14"/>
     </row>
     <row r="18" spans="1:14" ht="25" x14ac:dyDescent="0.15">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
       <c r="G18" s="46"/>
-      <c r="H18" s="66" t="s">
+      <c r="H18" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="66"/>
-      <c r="L18" s="66"/>
-      <c r="M18" s="66"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
       <c r="N18" s="11"/>
     </row>
     <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -1494,13 +1486,13 @@
       <c r="N19" s="15"/>
     </row>
     <row r="20" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="54" t="s">
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="70" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="26"/>
@@ -1515,19 +1507,19 @@
       <c r="K20" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="70" t="s">
+      <c r="L20" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="70"/>
+      <c r="M20" s="63"/>
       <c r="N20" s="15"/>
     </row>
     <row r="21" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="61"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
       <c r="G21" s="51"/>
       <c r="H21" s="36"/>
       <c r="I21" s="36"/>
@@ -1627,6 +1619,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A5:F8"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H5:M8"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="H11:M11"/>
@@ -1638,11 +1635,6 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="L20:M20"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A5:F8"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H5:M8"/>
   </mergeCells>
   <phoneticPr fontId="29" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
minor - focus A1
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/welcome.xlsx
+++ b/src/main/webapp/WEB-INF/book/welcome.xlsx
@@ -473,6 +473,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -520,9 +523,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1129,9 +1129,7 @@
   </sheetPr>
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1176,21 +1174,21 @@
       <c r="U1" s="1"/>
     </row>
     <row r="2" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
       <c r="N2" s="40"/>
     </row>
     <row r="3" spans="1:21" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -1226,87 +1224,87 @@
       <c r="N4" s="40"/>
     </row>
     <row r="5" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="65"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
       <c r="G5" s="44"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
       <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="65"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
       <c r="G6" s="45"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
       <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:21" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="65"/>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
       <c r="G7" s="45"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="65"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
       <c r="G8" s="45"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="70"/>
       <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:21" ht="25" x14ac:dyDescent="0.15">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
       <c r="G9" s="46"/>
-      <c r="H9" s="68" t="s">
+      <c r="H9" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="68"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
       <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:21" ht="25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1326,23 +1324,23 @@
       <c r="N10" s="12"/>
     </row>
     <row r="11" spans="1:21" ht="23" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="48"/>
-      <c r="H11" s="56" t="s">
+      <c r="H11" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
       <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:21" ht="29" customHeight="1" x14ac:dyDescent="0.15">
@@ -1351,10 +1349,10 @@
       <c r="C12" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="56"/>
       <c r="F12" s="18"/>
       <c r="G12" s="48"/>
       <c r="H12" s="19"/>
@@ -1362,10 +1360,10 @@
       <c r="J12" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="61" t="s">
+      <c r="K12" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="L12" s="61"/>
+      <c r="L12" s="62"/>
       <c r="M12" s="19"/>
       <c r="N12" s="12"/>
     </row>
@@ -1418,55 +1416,55 @@
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:21" ht="93" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
       <c r="G16" s="50"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
       <c r="N16" s="14"/>
     </row>
     <row r="17" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="57"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
       <c r="G17" s="50"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="61"/>
       <c r="N17" s="14"/>
     </row>
     <row r="18" spans="1:14" ht="25" x14ac:dyDescent="0.15">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="58"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
       <c r="G18" s="46"/>
-      <c r="H18" s="59" t="s">
+      <c r="H18" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
       <c r="N18" s="11"/>
     </row>
     <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.15">
@@ -1486,13 +1484,13 @@
       <c r="N19" s="15"/>
     </row>
     <row r="20" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="70" t="s">
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="54" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="26"/>
@@ -1507,19 +1505,19 @@
       <c r="K20" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="63" t="s">
+      <c r="L20" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="63"/>
+      <c r="M20" s="64"/>
       <c r="N20" s="15"/>
     </row>
     <row r="21" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="54"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
       <c r="G21" s="51"/>
       <c r="H21" s="36"/>
       <c r="I21" s="36"/>

</xml_diff>